<commit_message>
some window 70 data, started implementing IV estimation of stability measures. Am dealing with severe multicollinearity in the data though
</commit_message>
<xml_diff>
--- a/epidemic model/crisisPerSector.xlsx
+++ b/epidemic model/crisisPerSector.xlsx
@@ -24,15 +24,6 @@
     <t>Financial Crisis Dummy</t>
   </si>
   <si>
-    <t>NB</t>
-  </si>
-  <si>
-    <t>HNO</t>
-  </si>
-  <si>
-    <t>STG</t>
-  </si>
-  <si>
     <t>FG</t>
   </si>
   <si>
@@ -805,6 +796,15 @@
   </si>
   <si>
     <t>2015Q3</t>
+  </si>
+  <si>
+    <t>NFB</t>
+  </si>
+  <si>
+    <t>HH&amp;NP</t>
+  </si>
+  <si>
+    <t>S&amp;LG</t>
   </si>
 </sst>
 </file>
@@ -844,7 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -860,9 +860,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -900,7 +900,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -972,7 +972,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1125,7 +1125,7 @@
   <dimension ref="A1:G256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,27 +1135,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -2029,7 +2029,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -2236,7 +2236,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -2673,7 +2673,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -2857,7 +2857,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -2949,7 +2949,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -3202,7 +3202,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -3340,7 +3340,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -3363,7 +3363,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -3455,7 +3455,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -3478,7 +3478,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -3524,7 +3524,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -3547,7 +3547,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -3616,7 +3616,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -3685,7 +3685,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -3754,7 +3754,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -3800,7 +3800,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -3846,7 +3846,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -3961,7 +3961,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -3984,7 +3984,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -4007,7 +4007,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -4099,7 +4099,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -4122,7 +4122,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -4145,7 +4145,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -4168,7 +4168,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -4191,7 +4191,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -4260,7 +4260,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -4283,7 +4283,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -4352,7 +4352,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -4375,7 +4375,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -4398,7 +4398,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -4421,7 +4421,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -4467,7 +4467,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -4559,7 +4559,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -4582,7 +4582,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -4628,7 +4628,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -4674,7 +4674,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -4743,7 +4743,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -4766,7 +4766,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -4789,7 +4789,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -4812,7 +4812,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -4835,7 +4835,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -4858,7 +4858,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -4904,7 +4904,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -4927,7 +4927,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -4950,7 +4950,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -4973,7 +4973,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -5019,7 +5019,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -5042,7 +5042,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -5065,7 +5065,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -5111,7 +5111,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -5134,7 +5134,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -5157,7 +5157,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B176">
         <v>1</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -5203,7 +5203,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -5226,7 +5226,7 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -5249,7 +5249,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -5272,7 +5272,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -5295,7 +5295,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -5318,7 +5318,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -5341,7 +5341,7 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -5364,7 +5364,7 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -5387,7 +5387,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -5410,7 +5410,7 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -5456,7 +5456,7 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -5479,7 +5479,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -5525,7 +5525,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -5571,7 +5571,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -5594,7 +5594,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -5617,7 +5617,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -5640,7 +5640,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -5663,7 +5663,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B198">
         <v>1</v>
@@ -5686,7 +5686,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -5709,7 +5709,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -5732,7 +5732,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -5755,7 +5755,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -5778,7 +5778,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -5824,7 +5824,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -5847,7 +5847,7 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B206">
         <v>1</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -5916,7 +5916,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -5939,7 +5939,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B210">
         <v>1</v>
@@ -5962,7 +5962,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -5985,7 +5985,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -6008,7 +6008,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B213">
         <v>1</v>
@@ -6031,7 +6031,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B214">
         <v>1</v>
@@ -6054,7 +6054,7 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -6077,7 +6077,7 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -6100,7 +6100,7 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -6123,7 +6123,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B218">
         <v>1</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B219">
         <v>1</v>
@@ -6169,7 +6169,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -6192,7 +6192,7 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -6215,7 +6215,7 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -6238,7 +6238,7 @@
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -6261,7 +6261,7 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B225">
         <v>0</v>
@@ -6307,7 +6307,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -6330,7 +6330,7 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -6353,7 +6353,7 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -6376,7 +6376,7 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -6399,7 +6399,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -6422,7 +6422,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -6445,7 +6445,7 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -6491,7 +6491,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -6514,7 +6514,7 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -6537,7 +6537,7 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -6560,7 +6560,7 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B237">
         <v>1</v>
@@ -6583,7 +6583,7 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B238">
         <v>1</v>
@@ -6606,7 +6606,7 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B239">
         <v>1</v>
@@ -6629,7 +6629,7 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B241">
         <v>0</v>
@@ -6675,7 +6675,7 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -6698,7 +6698,7 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -6721,7 +6721,7 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -6744,7 +6744,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -6767,7 +6767,7 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -6790,7 +6790,7 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -6813,7 +6813,7 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B248">
         <v>1</v>
@@ -6836,7 +6836,7 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B249">
         <v>1</v>
@@ -6859,7 +6859,7 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B250">
         <v>1</v>
@@ -6882,7 +6882,7 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B251">
         <v>1</v>
@@ -6905,7 +6905,7 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B252">
         <v>1</v>
@@ -6928,7 +6928,7 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -6951,7 +6951,7 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B254">
         <v>1</v>
@@ -6974,7 +6974,7 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -6997,7 +6997,7 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -7024,6 +7024,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D156EDECDFFA04389F38E90B325C883" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7c04d2d39ad5b5759ef8ba5679918ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0343a904-03a6-4420-a0c7-59ff8ba6adb7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10c043409dcd935feb895d13645ae8c9" ns2:_="">
     <xsd:import namespace="0343a904-03a6-4420-a0c7-59ff8ba6adb7"/>
@@ -7171,29 +7186,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F09E5E9-A7CB-40C3-98D0-BC0B57911982}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB215A86-6080-4206-8E99-8F14EFDCC964}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6778B81-693E-45AD-838D-46215E8B9E18}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6778B81-693E-45AD-838D-46215E8B9E18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB215A86-6080-4206-8E99-8F14EFDCC964}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F09E5E9-A7CB-40C3-98D0-BC0B57911982}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0343a904-03a6-4420-a0c7-59ff8ba6adb7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>